<commit_message>
PCB Update and Purchase List
</commit_message>
<xml_diff>
--- a/Parça Listesi.xlsx
+++ b/Parça Listesi.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emir\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emir\Desktop\MiniMiniRobots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0C2FDF5-0798-4523-92BD-07D894C514B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58FE2E64-8984-4644-8B54-5E74C66376CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE449F72-0D21-42EC-9291-6FD36F8710DD}"/>
   </bookViews>
@@ -36,141 +36,123 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Parça</t>
   </si>
   <si>
-    <t>Açıklama</t>
-  </si>
-  <si>
     <t>Adet</t>
   </si>
   <si>
     <t>Link</t>
   </si>
   <si>
-    <t>Kontrolcü</t>
-  </si>
-  <si>
     <t>Raspberry Pi Pico W</t>
   </si>
   <si>
-    <t>https://www.direnc.net/raspberry-pi-pico-w</t>
-  </si>
-  <si>
-    <t>Step Motor ve Sürücü</t>
-  </si>
-  <si>
-    <t>28 BYJ-48 Redüktörlü Step Motor ve ULN2003A</t>
-  </si>
-  <si>
-    <t>https://www.direnc.net/28-byj-48-reduktorlu-step-motor-ve-uln2003a-step-motor-surucu-karti</t>
-  </si>
-  <si>
-    <t>DC Motor Sürücü</t>
-  </si>
-  <si>
-    <t>L293D</t>
-  </si>
-  <si>
-    <t>https://ozdisan.com/integrated-circuits-ics/power-management-ics/power-drivers/L293D/615433</t>
-  </si>
-  <si>
-    <t>Buck Converter</t>
-  </si>
-  <si>
-    <t>AMS1117 Modül 5V</t>
-  </si>
-  <si>
-    <t>https://www.direnc.net/ams1117-5v-modul</t>
-  </si>
-  <si>
-    <t>Header</t>
-  </si>
-  <si>
-    <t>1x20 Female Header 2.54mm</t>
-  </si>
-  <si>
-    <t>https://ozdisan.com/connectors-and-interconnects/headers/female-headers/DS1023-1X20S22/358345</t>
-  </si>
-  <si>
-    <t>Pico Header</t>
-  </si>
-  <si>
-    <t>Step Motor Connecter</t>
-  </si>
-  <si>
-    <t>CON.T.B.2.50MM 5PIN(1X5) 90C MALE</t>
-  </si>
-  <si>
-    <t>https://ozdisan.com/connectors-and-interconnects/rectangular-connectors/pcb-connectors/L-KLS1-XL4-2-50-05-R/515839</t>
-  </si>
-  <si>
-    <t>DC Motor and Power Supply Connecter</t>
-  </si>
-  <si>
-    <t>TERM.BLK.5.00MM 2P</t>
-  </si>
-  <si>
-    <t>https://ozdisan.com/connectors-and-interconnects/terminal-blocks/pcb-terminal-blocks/DG126-5-0-02P-14-00AH/361882</t>
-  </si>
-  <si>
-    <t>Neopixel Connecter</t>
-  </si>
-  <si>
-    <t>TERM.BLK.5.00MM 3P</t>
-  </si>
-  <si>
-    <t>https://ozdisan.com/connectors-and-interconnects/terminal-blocks/pcb-terminal-blocks/DG126-5-0-03P-14-00AH/361883</t>
-  </si>
-  <si>
-    <t>Reset Butonu</t>
-  </si>
-  <si>
-    <t>6x6 4.3mm Tach Buton (2 Bacak</t>
-  </si>
-  <si>
-    <t>https://www.direnc.net/6x6-43mm-tach-buton-2-bacak</t>
-  </si>
-  <si>
-    <t>1x40 12mm Erkek Header</t>
-  </si>
-  <si>
-    <t>https://www.direnc.net/1x40-12mm-erkek-header-1</t>
-  </si>
-  <si>
-    <t>20k Ohm Direnç</t>
-  </si>
-  <si>
-    <t>10k Ohm Direnç</t>
-  </si>
-  <si>
-    <t>Direnç</t>
-  </si>
-  <si>
     <t>https://www.robotistan.com/14w-20k-direnc-paketi-10-adet</t>
   </si>
   <si>
     <t>https://www.robotistan.com/14w-10k-direnc-paketi-10-adet</t>
   </si>
   <si>
-    <t>Kondansatör</t>
-  </si>
-  <si>
-    <t>10uF Kondansatör</t>
-  </si>
-  <si>
     <t>https://www.robotistan.com/10-uf-16-v-elektrolit-kondansator</t>
   </si>
   <si>
-    <t>Şarj Devresi</t>
-  </si>
-  <si>
-    <t>https://www.robitshop.com/urun/2s-3a-lityum-batarya-bms-balans-karti-18650-pil-sarji-icin-uygun</t>
-  </si>
-  <si>
-    <t>2S 3A Lityum Batarya BMS Balans Kartı</t>
+    <t>NeoPixel 8′li Şerit</t>
+  </si>
+  <si>
+    <t>https://www.robolinkmarket.com/neopixel-8li-serit</t>
+  </si>
+  <si>
+    <t>LM2596 Ayarlanabilir DC/DC Voltaj Regülatörü</t>
+  </si>
+  <si>
+    <t>https://www.robolinkmarket.com/raspberry-pi-pico-w</t>
+  </si>
+  <si>
+    <t>https://www.robolinkmarket.com/1x8-pin-disi-header-siyah</t>
+  </si>
+  <si>
+    <t>1x8 Pin Dişi Header - Siyah</t>
+  </si>
+  <si>
+    <t>1x4 Pin Dişi Header - Siyah</t>
+  </si>
+  <si>
+    <t>https://www.robolinkmarket.com/1x4-pin-disi-header-siyah</t>
+  </si>
+  <si>
+    <t>https://www.robolinkmarket.com/28byj-48-step-motor-ve-uln2003-surucu</t>
+  </si>
+  <si>
+    <t>28BYJ-48 Step Motor ve Uln2003 Sürücü</t>
+  </si>
+  <si>
+    <t>L293D Motor Sürücü</t>
+  </si>
+  <si>
+    <t>https://www.robolinkmarket.com/l293d-motor-surucu</t>
+  </si>
+  <si>
+    <t>https://www.robolinkmarket.com/lm2596-ayarlanabilir-dc-dc-voltaj-regulatoru</t>
+  </si>
+  <si>
+    <t>2 Pin 5mm Terminal Klemens</t>
+  </si>
+  <si>
+    <t>https://www.robolinkmarket.com/2-pin-5mm-terminal-konnektor</t>
+  </si>
+  <si>
+    <t>3 Pin 5mm Terminal Klemens</t>
+  </si>
+  <si>
+    <t>https://www.robolinkmarket.com/3-pin-5mm-terminal-konnektor</t>
+  </si>
+  <si>
+    <t>2 Pinli Tact Buton - 6x6mm</t>
+  </si>
+  <si>
+    <t>https://www.robolinkmarket.com/2-pinli-tact-buton-6x6mm</t>
+  </si>
+  <si>
+    <t>40 Pin Erkek Header</t>
+  </si>
+  <si>
+    <t>https://www.robolinkmarket.com/40-pin-erkek-header</t>
+  </si>
+  <si>
+    <t>2S 5A BMS - Batarya Yönetim ve Koruma Modülü</t>
+  </si>
+  <si>
+    <t>https://www.robolinkmarket.com/2s-5a-bms-batarya-yonetim-ve-koruma-modulu</t>
+  </si>
+  <si>
+    <t>2'li AA Pil Yuvası</t>
+  </si>
+  <si>
+    <t>https://www.robolinkmarket.com/2li-aa-pil-yuvasi</t>
+  </si>
+  <si>
+    <t>0.96 inch I2C OLED Ekran 128x64-Mavi/Siyah</t>
+  </si>
+  <si>
+    <t>https://www.robolinkmarket.com/096-i2c-oled-128x64-4pin-blue-black</t>
+  </si>
+  <si>
+    <t>JST-XH 2.54mm Soketli 5 Pin Eğik Tunik Konnektör</t>
+  </si>
+  <si>
+    <t>https://www.robotistan.com/jstxh-254mm-egik-5pin-konnektor</t>
+  </si>
+  <si>
+    <t>1/4 W 20K Direnç Paketi - 10 Adet</t>
+  </si>
+  <si>
+    <t>1/4 W 10K Direnç Paketi - 10 Adet</t>
+  </si>
+  <si>
+    <t>10 uF 16 V Elektrolit Kondansatör</t>
   </si>
 </sst>
 </file>
@@ -539,21 +521,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EEEB3B7-20B5-497F-A08E-D630C31CE465}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="111.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="111.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -563,224 +544,217 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="1">
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1">
         <v>3</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="C9" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="1">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="1">
         <v>2</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="1">
-        <v>3</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="C16" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="1">
+      <c r="B19" s="1">
         <v>2</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>43</v>
+      <c r="C19" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D12" r:id="rId1" xr:uid="{81600A5E-6211-456A-B907-64DE83C4CE9C}"/>
-    <hyperlink ref="D13" r:id="rId2" xr:uid="{EB9E37E6-B291-42D1-B2B5-4CA93F941193}"/>
-    <hyperlink ref="D11" r:id="rId3" xr:uid="{8DA86BA9-AE33-4C11-BC12-A625EE02014A}"/>
-    <hyperlink ref="D10" r:id="rId4" xr:uid="{26C88BFA-D636-478B-AD4C-0FD4D4E013BC}"/>
-    <hyperlink ref="D9" r:id="rId5" xr:uid="{C5E370E7-8690-46AF-BC91-E4A001C39C04}"/>
-    <hyperlink ref="D8" r:id="rId6" xr:uid="{5530BE01-C7BF-4A31-B36C-3ADE13729FA9}"/>
-    <hyperlink ref="D7" r:id="rId7" xr:uid="{A5662ED8-27B3-4BF2-BC94-2F8E5F3D17CC}"/>
-    <hyperlink ref="D2" r:id="rId8" xr:uid="{B8B4A574-56DE-4E07-BA12-89892135DE18}"/>
-    <hyperlink ref="D3" r:id="rId9" xr:uid="{4D3EE5BA-9DC6-4706-A5F0-725F14C5AE05}"/>
-    <hyperlink ref="D4" r:id="rId10" xr:uid="{145356EC-C736-4462-8BC8-31FB13851CBA}"/>
-    <hyperlink ref="D5" r:id="rId11" xr:uid="{57F11DFC-D376-4B8C-A67F-A8AC36EED7EE}"/>
-    <hyperlink ref="D6" r:id="rId12" xr:uid="{101E06F4-F093-468A-86BF-029610FAEA76}"/>
-    <hyperlink ref="D14" r:id="rId13" xr:uid="{037CB538-758A-49A2-836C-54B92422427A}"/>
-    <hyperlink ref="D15" r:id="rId14" xr:uid="{A3AEF786-E7E9-4B48-8F0E-61E73497E5E9}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{0134B681-7EA0-4472-B45F-13FB855C9774}"/>
+    <hyperlink ref="C7" r:id="rId2" xr:uid="{B66EE9AC-3AFC-40A5-AC19-B9B2207D0CB4}"/>
+    <hyperlink ref="C10" r:id="rId3" xr:uid="{34728CA2-65CC-4218-8D2A-9FFE6E360DF3}"/>
+    <hyperlink ref="C11" r:id="rId4" xr:uid="{C773E7BD-4DFA-464A-B090-B6D31116947F}"/>
+    <hyperlink ref="C12" r:id="rId5" xr:uid="{3870229D-C88C-47D7-82C3-3D56108F2CA5}"/>
+    <hyperlink ref="C5" r:id="rId6" xr:uid="{1D410FD0-1723-4AA5-8DC3-55E9B6E689E6}"/>
+    <hyperlink ref="C13" r:id="rId7" xr:uid="{0D5F98A3-6F60-404B-A95C-8C2114EDEA25}"/>
+    <hyperlink ref="C16" r:id="rId8" xr:uid="{FF36C161-8678-46ED-8C76-28D927337E98}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>